<commit_message>
Update templates and handle empty rows and user input error
</commit_message>
<xml_diff>
--- a/data/docs/bulk-submissions/NMDC-EDGE-Metagenomics-ReadsQC-bulk-submission.xlsx
+++ b/data/docs/bulk-submissions/NMDC-EDGE-Metagenomics-ReadsQC-bulk-submission.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yxu/dev/node16_apps/nmdc-edge/data/docs/bulk-submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03551E5-C71C-7C42-B0F6-CD1491036C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C14CEA2-552C-3E49-8764-2334363C1E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16620" yWindow="8200" windowWidth="27240" windowHeight="16440" xr2:uid="{D4B1EDC8-DFE1-D14C-9E75-173BCE7BAFAC}"/>
+    <workbookView xWindow="1100" yWindow="2840" windowWidth="27240" windowHeight="16440" xr2:uid="{D4B1EDC8-DFE1-D14C-9E75-173BCE7BAFAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,13 +50,13 @@
     <t>Sequencing Platform</t>
   </si>
   <si>
-    <t>Paired-end Illumina/PacBio FASTQ</t>
-  </si>
-  <si>
-    <t>Illumina Pair-1 FASTQ</t>
-  </si>
-  <si>
-    <t>Illumina Pair-2 FASTQ</t>
+    <t>Illumina Paired-end R1 FASTQ</t>
+  </si>
+  <si>
+    <t>Interleaved or Single-end Illumina/PacBio FASTQ</t>
+  </si>
+  <si>
+    <t>Illumina Paired-end  R2  FASTQ</t>
   </si>
 </sst>
 </file>
@@ -92,11 +92,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,17 +428,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{030A96EA-2FA1-8348-B17F-A091C9D7BE5F}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="33.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" customWidth="1"/>
-    <col min="5" max="5" width="34" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.1640625" customWidth="1"/>
+    <col min="3" max="3" width="41" customWidth="1"/>
+    <col min="4" max="5" width="31.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -452,10 +449,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -463,21 +460,18 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C2" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Project/Run Name" error="Invalid Input" promptTitle="Project/Run Name" prompt="Required. At least 3 but less than 30 characters. Only alphabets, numbers, dashs, dot and underscore are allowed." sqref="A2:A100" xr:uid="{291FD160-E4F0-854B-9418-A6B8EACE1298}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Illumina R1 FASTQ" prompt="Accept uploaded files, Retrieved SRA files and http(s) url inputs. Separate multiple files with commas._x000a__x000a_Examples:_x000a_upload/test_R1.fq_x000a_sra/SRR30724627_1.fastq.gz_x000a_https://nmdc-edge.org/publicdata/test_data/Ecoli_10x.1.fastq" sqref="D2:D99" xr:uid="{5FCBE9B3-9D75-384A-9086-4A4CE3DAB6D7}"/>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Project/Run Name" error="Invalid Input" promptTitle="Project/Run Name" prompt="Required. At least 3 but less than 30 characters. Only alphabets, numbers, dashs, dot and underscore are allowed." sqref="A2:A99" xr:uid="{291FD160-E4F0-854B-9418-A6B8EACE1298}">
       <formula1>3</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Description" prompt="Optional" sqref="B2:B100" xr:uid="{CB3D86F2-D212-C340-9296-8EF1CAF1D742}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Illumina Pair-1 FASTQ" prompt="Accept uploaded files, SRA files and http(s) url inputs. Separate multiple files with commas._x000a__x000a_Examples:_x000a_upload/test_R1.fq_x000a_sra/SRR1602702.fastq.gz_x000a_https://nmdc-edge.org/publicdata/test_data/Ecoli_interleaved_pe_small.fastq" sqref="D2:D100" xr:uid="{5FCBE9B3-9D75-384A-9086-4A4CE3DAB6D7}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Illumina Pair-2 FASTQ" prompt="Accept uploaded files, SRA files and http(s) url inputs. Separate multiple files with commas._x000a__x000a_Examples:_x000a_upload/test_R1.fq_x000a_sra/SRR1602702.fastq.gz_x000a_https://nmdc-edge.org/publicdata/test_data/Ecoli_interleaved_pe_small.fastq" sqref="E2:E100" xr:uid="{9667BBE3-FF05-1C4F-A787-AC2369651A5F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Paired-end Illumina/PacBio FASTQ" prompt="Accept uploaded files, SRA files and http(s) url inputs. Separate multiple files with commas._x000a__x000a_Examples:_x000a_upload/test_R1.fq_x000a_sra/SRR1602702.fastq.gz_x000a_https://nmdc-edge.org/publicdata/test_data/Ecoli_interleaved_pe_small.fastq" sqref="C2:C100" xr:uid="{776E149A-8CE7-8742-B499-CD03793E3956}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sequencing Platform" prompt="Default: Illumina" sqref="F2:F100" xr:uid="{61037986-14E0-8444-AAEF-DD8847150EB9}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Description" prompt="Optional" sqref="B2:B99" xr:uid="{CB3D86F2-D212-C340-9296-8EF1CAF1D742}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Illumina R2 FASTQ" prompt="Accept uploaded files, Retrieved SRA files and http(s) url inputs. Separate multiple files with commas._x000a__x000a_Examples:_x000a_upload/test_R2.fq_x000a_sra/SRR30724627_2.fastq.gz_x000a_https://nmdc-edge.org/publicdata/test_data/Ecoli_10x.2.fastq" sqref="E2:E99" xr:uid="{9667BBE3-FF05-1C4F-A787-AC2369651A5F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Single Illumina/PacBio FASTQ" prompt="Accept uploaded files, Retrieved SRA files and http(s) url inputs. Separate multiple files with commas._x000a__x000a_Examples:_x000a_upload/test_R1.fq_x000a_sra/SRR1602702.fastq.gz_x000a_https://nmdc-edge.org/publicdata/test_data/Ecoli_interleaved_pe_small.fastq" sqref="C2:C99" xr:uid="{776E149A-8CE7-8742-B499-CD03793E3956}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sequencing Platform" prompt="Default: Illumina" sqref="F2:F99" xr:uid="{5CC4AEE4-243A-134C-BDF1-AC25E7FBD780}">
       <formula1>"Illumina, PacBio"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add "Data Source" column to template
</commit_message>
<xml_diff>
--- a/data/docs/bulk-submissions/NMDC-EDGE-Metagenomics-ReadsQC-bulk-submission.xlsx
+++ b/data/docs/bulk-submissions/NMDC-EDGE-Metagenomics-ReadsQC-bulk-submission.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yxu/dev/node16_apps/nmdc-edge/data/docs/bulk-submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C14CEA2-552C-3E49-8764-2334363C1E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CEA201-D16B-B043-BFDA-82516EA749DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="2840" windowWidth="27240" windowHeight="16440" xr2:uid="{D4B1EDC8-DFE1-D14C-9E75-173BCE7BAFAC}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Project/Run Name</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Illumina Paired-end  R2  FASTQ</t>
+  </si>
+  <si>
+    <t>Data Source</t>
   </si>
 </sst>
 </file>
@@ -428,20 +431,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{030A96EA-2FA1-8348-B17F-A091C9D7BE5F}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.1640625" customWidth="1"/>
-    <col min="3" max="3" width="41" customWidth="1"/>
-    <col min="4" max="5" width="31.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.5" customWidth="1"/>
+    <col min="2" max="3" width="32.1640625" customWidth="1"/>
+    <col min="4" max="4" width="41" customWidth="1"/>
+    <col min="5" max="6" width="31.6640625" customWidth="1"/>
+    <col min="7" max="7" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,31 +452,38 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Illumina R1 FASTQ" prompt="Accept uploaded files, Retrieved SRA files and http(s) url inputs. Separate multiple files with commas._x000a__x000a_Examples:_x000a_upload/test_R1.fq_x000a_sra/SRR30724627_1.fastq.gz_x000a_https://nmdc-edge.org/publicdata/test_data/Ecoli_10x.1.fastq" sqref="D2:D99" xr:uid="{5FCBE9B3-9D75-384A-9086-4A4CE3DAB6D7}"/>
+  <dataValidations count="8">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Illumina R1 FASTQ" prompt="Omit this column if input is Single fastq_x000a__x000a_Enter file name if Data Source is Uploaded File or Retrieved SRA Data_x000a__x000a_Enter file url if Data Source is HTTP(s) URL_x000a__x000a_Separate multiple inputs with commas" sqref="E2:E99" xr:uid="{5FCBE9B3-9D75-384A-9086-4A4CE3DAB6D7}"/>
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Project/Run Name" error="Invalid Input" promptTitle="Project/Run Name" prompt="Required. At least 3 but less than 30 characters. Only alphabets, numbers, dashs, dot and underscore are allowed." sqref="A2:A99" xr:uid="{291FD160-E4F0-854B-9418-A6B8EACE1298}">
       <formula1>3</formula1>
       <formula2>30</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Description" prompt="Optional" sqref="B2:B99" xr:uid="{CB3D86F2-D212-C340-9296-8EF1CAF1D742}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Illumina R2 FASTQ" prompt="Accept uploaded files, Retrieved SRA files and http(s) url inputs. Separate multiple files with commas._x000a__x000a_Examples:_x000a_upload/test_R2.fq_x000a_sra/SRR30724627_2.fastq.gz_x000a_https://nmdc-edge.org/publicdata/test_data/Ecoli_10x.2.fastq" sqref="E2:E99" xr:uid="{9667BBE3-FF05-1C4F-A787-AC2369651A5F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Single Illumina/PacBio FASTQ" prompt="Accept uploaded files, Retrieved SRA files and http(s) url inputs. Separate multiple files with commas._x000a__x000a_Examples:_x000a_upload/test_R1.fq_x000a_sra/SRR1602702.fastq.gz_x000a_https://nmdc-edge.org/publicdata/test_data/Ecoli_interleaved_pe_small.fastq" sqref="C2:C99" xr:uid="{776E149A-8CE7-8742-B499-CD03793E3956}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sequencing Platform" prompt="Default: Illumina" sqref="F2:F99" xr:uid="{5CC4AEE4-243A-134C-BDF1-AC25E7FBD780}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Illumina R2 FASTQ" prompt="Omit this column if input is Single fastq_x000a__x000a_Enter file name if Data Source is Uploaded File or Retrieved SRA Data_x000a__x000a_Enter file url if Data Source is HTTP(s) URL_x000a__x000a_Separate multiple inputs with commas" sqref="F3:F99" xr:uid="{9667BBE3-FF05-1C4F-A787-AC2369651A5F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Single Illumina/PacBio FASTQ" prompt="Omit this column if input is Paired-end fastq_x000a__x000a_Enter file name if Data Source is Uploaded File or Retrieved SRA Data_x000a__x000a_Enter file url if Data Source is HTTP(s) URL_x000a__x000a_Separate multiple inputs with commas" sqref="D2:D99" xr:uid="{776E149A-8CE7-8742-B499-CD03793E3956}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sequencing Platform" prompt="Default: Illumina" sqref="G2:G99" xr:uid="{5CC4AEE4-243A-134C-BDF1-AC25E7FBD780}">
       <formula1>"Illumina, PacBio"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data Source" prompt="Default: Uploaded File" sqref="C2:C108" xr:uid="{CBEA70A8-438C-B741-BF37-86C351AB6956}">
+      <formula1>"Uploaded File, Retrieved SRA Data, HTTP(s) URL"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Illumina R2 FASTQ" prompt="Omit this column if input is Single fastq_x000a__x000a_Enter file name if Data Source is Uploaded File or Retrieved SRA Data_x000a__x000a_Enter file url if Data Source is HTTP(s) URL_x000a__x000a_Separate multiple inputs with commas" sqref="F2 F3" xr:uid="{E45419E6-3A65-4048-B1DF-0884CD2DE488}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bulk submission template
</commit_message>
<xml_diff>
--- a/data/docs/bulk-submissions/NMDC-EDGE-Metagenomics-ReadsQC-bulk-submission.xlsx
+++ b/data/docs/bulk-submissions/NMDC-EDGE-Metagenomics-ReadsQC-bulk-submission.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yxu/dev/node16_apps/nmdc-edge/data/docs/bulk-submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CEA201-D16B-B043-BFDA-82516EA749DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3357C53-B7C9-0448-8084-5768B610D8D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="2840" windowWidth="27240" windowHeight="16440" xr2:uid="{D4B1EDC8-DFE1-D14C-9E75-173BCE7BAFAC}"/>
+    <workbookView xWindow="8620" yWindow="8360" windowWidth="27240" windowHeight="16440" xr2:uid="{D4B1EDC8-DFE1-D14C-9E75-173BCE7BAFAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -439,9 +439,9 @@
   <cols>
     <col min="1" max="1" width="29.33203125" customWidth="1"/>
     <col min="2" max="3" width="32.1640625" customWidth="1"/>
-    <col min="4" max="4" width="41" customWidth="1"/>
-    <col min="5" max="6" width="31.6640625" customWidth="1"/>
-    <col min="7" max="7" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="41" customWidth="1"/>
+    <col min="6" max="7" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -455,35 +455,34 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="8">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Illumina R1 FASTQ" prompt="Omit this column if input is Single fastq_x000a__x000a_Enter file name if Data Source is Uploaded File or Retrieved SRA Data_x000a__x000a_Enter file url if Data Source is HTTP(s) URL_x000a__x000a_Separate multiple inputs with commas" sqref="E2:E99" xr:uid="{5FCBE9B3-9D75-384A-9086-4A4CE3DAB6D7}"/>
+  <dataValidations count="7">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Illumina R1 FASTQ" prompt="Omit this column if input is Single fastq_x000a__x000a_Enter file name if Data Source is Uploaded File or Retrieved SRA Data_x000a__x000a_Enter file url if Data Source is HTTP(s) URL_x000a__x000a_Separate multiple inputs with commas" sqref="F2:F99" xr:uid="{5FCBE9B3-9D75-384A-9086-4A4CE3DAB6D7}"/>
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Project/Run Name" error="Invalid Input" promptTitle="Project/Run Name" prompt="Required. At least 3 but less than 30 characters. Only alphabets, numbers, dashs, dot and underscore are allowed." sqref="A2:A99" xr:uid="{291FD160-E4F0-854B-9418-A6B8EACE1298}">
       <formula1>3</formula1>
       <formula2>30</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Description" prompt="Optional" sqref="B2:B99" xr:uid="{CB3D86F2-D212-C340-9296-8EF1CAF1D742}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Illumina R2 FASTQ" prompt="Omit this column if input is Single fastq_x000a__x000a_Enter file name if Data Source is Uploaded File or Retrieved SRA Data_x000a__x000a_Enter file url if Data Source is HTTP(s) URL_x000a__x000a_Separate multiple inputs with commas" sqref="F3:F99" xr:uid="{9667BBE3-FF05-1C4F-A787-AC2369651A5F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Single Illumina/PacBio FASTQ" prompt="Omit this column if input is Paired-end fastq_x000a__x000a_Enter file name if Data Source is Uploaded File or Retrieved SRA Data_x000a__x000a_Enter file url if Data Source is HTTP(s) URL_x000a__x000a_Separate multiple inputs with commas" sqref="D2:D99" xr:uid="{776E149A-8CE7-8742-B499-CD03793E3956}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sequencing Platform" prompt="Default: Illumina" sqref="G2:G99" xr:uid="{5CC4AEE4-243A-134C-BDF1-AC25E7FBD780}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Illumina R2 FASTQ" prompt="Omit this column if input is Single fastq_x000a__x000a_Enter file name if Data Source is Uploaded File or Retrieved SRA Data_x000a__x000a_Enter file url if Data Source is HTTP(s) URL_x000a__x000a_Separate multiple inputs with commas" sqref="G2:G99" xr:uid="{9667BBE3-FF05-1C4F-A787-AC2369651A5F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Single Illumina/PacBio FASTQ" prompt="Omit this column if input is Paired-end fastq_x000a__x000a_Enter file name if Data Source is Uploaded File or Retrieved SRA Data_x000a__x000a_Enter file url if Data Source is HTTP(s) URL_x000a__x000a_Separate multiple inputs with commas" sqref="E2:E99" xr:uid="{776E149A-8CE7-8742-B499-CD03793E3956}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sequencing Platform" error="Select from dropdown list" promptTitle="Sequencing Platform" prompt="Default: Illumina" sqref="D2:D99" xr:uid="{5CC4AEE4-243A-134C-BDF1-AC25E7FBD780}">
       <formula1>"Illumina, PacBio"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data Source" prompt="Default: Uploaded File" sqref="C2:C108" xr:uid="{CBEA70A8-438C-B741-BF37-86C351AB6956}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Data Source" error="Select from dropdown list" promptTitle="Data Source" prompt="Default: Uploaded File" sqref="C2:D108" xr:uid="{CBEA70A8-438C-B741-BF37-86C351AB6956}">
       <formula1>"Uploaded File, Retrieved SRA Data, HTTP(s) URL"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Illumina R2 FASTQ" prompt="Omit this column if input is Single fastq_x000a__x000a_Enter file name if Data Source is Uploaded File or Retrieved SRA Data_x000a__x000a_Enter file url if Data Source is HTTP(s) URL_x000a__x000a_Separate multiple inputs with commas" sqref="F2 F3" xr:uid="{E45419E6-3A65-4048-B1DF-0884CD2DE488}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>